<commit_message>
updates and new posts
</commit_message>
<xml_diff>
--- a/assets/AdditionalParts.xlsx
+++ b/assets/AdditionalParts.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="48">
   <si>
     <t xml:space="preserve">das musicding</t>
   </si>
@@ -35,6 +35,9 @@
   </si>
   <si>
     <t xml:space="preserve">Location</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://nl.rs-online.com/web/</t>
   </si>
   <si>
     <t xml:space="preserve">10k</t>
@@ -170,11 +173,12 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -197,14 +201,10 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
@@ -253,7 +253,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -270,11 +270,7 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -295,21 +291,22 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:M30"/>
+  <dimension ref="A1:N30"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A8" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J26" activeCellId="0" sqref="J26"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E4" activeCellId="0" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="13.4285714285714"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="11.5204081632653"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="15.3979591836735"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="16.8112244897959"/>
-    <col collapsed="false" hidden="false" max="8" min="5" style="1" width="11.5204081632653"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="19.6275510204082"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="1" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="13.2295918367347"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="15.2551020408163"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="16.6020408163265"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="24.7142857142857"/>
+    <col collapsed="false" hidden="false" max="9" min="6" style="1" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="19.3061224489796"/>
+    <col collapsed="false" hidden="false" max="1025" min="11" style="1" width="11.3418367346939"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -330,38 +327,41 @@
       <c r="D2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="3" t="s">
-        <v>1</v>
+      <c r="E2" s="1" t="s">
+        <v>5</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I2" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="J2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="J2" s="3"/>
+      <c r="K2" s="3"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="n">
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="G3" s="1" t="n">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="H3" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="I3" s="1" t="s">
-        <v>8</v>
+        <v>2</v>
+      </c>
+      <c r="I3" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -369,30 +369,30 @@
         <v>2</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="G4" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="H4" s="1" t="s">
         <v>11</v>
+      </c>
+      <c r="H4" s="1" t="n">
+        <v>1</v>
       </c>
       <c r="I4" s="1" t="s">
         <v>12</v>
       </c>
+      <c r="J4" s="1" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="G5" s="1" t="n">
-        <v>2</v>
-      </c>
       <c r="H5" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="I5" s="1" t="n">
         <v>470</v>
       </c>
-      <c r="I5" s="1" t="s">
-        <v>12</v>
+      <c r="J5" s="1" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -400,228 +400,199 @@
         <v>2</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="G6" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="H6" s="1" t="s">
         <v>16</v>
       </c>
+      <c r="H6" s="1" t="n">
+        <v>2</v>
+      </c>
       <c r="I6" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="K7" s="4"/>
-      <c r="L7" s="4"/>
-      <c r="M7" s="4"/>
+        <v>17</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="n">
         <v>2</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="G8" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="H8" s="1" t="s">
         <v>18</v>
       </c>
+      <c r="H8" s="1" t="n">
+        <v>1</v>
+      </c>
       <c r="I8" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="K8" s="4"/>
-      <c r="L8" s="4"/>
-      <c r="M8" s="4"/>
+        <v>19</v>
+      </c>
+      <c r="J8" s="1" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="n">
         <v>1</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="G9" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="H9" s="1" t="s">
-        <v>5</v>
+        <v>20</v>
+      </c>
+      <c r="H9" s="1" t="n">
+        <v>1</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="K9" s="4"/>
-      <c r="L9" s="5"/>
-      <c r="M9" s="5"/>
+        <v>6</v>
+      </c>
+      <c r="J9" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="M9" s="4"/>
+      <c r="N9" s="4"/>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="G10" s="4" t="n">
-        <v>2</v>
-      </c>
-      <c r="H10" s="4" t="n">
+      <c r="H10" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="I10" s="1" t="n">
         <v>820</v>
       </c>
-      <c r="I10" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="K10" s="4"/>
-      <c r="L10" s="4"/>
-      <c r="M10" s="4"/>
+      <c r="J10" s="1" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="n">
         <v>1</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="G11" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="H11" s="1" t="s">
         <v>23</v>
       </c>
+      <c r="H11" s="1" t="n">
+        <v>1</v>
+      </c>
       <c r="I11" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="K11" s="4"/>
-      <c r="L11" s="4"/>
-      <c r="M11" s="4"/>
+        <v>24</v>
+      </c>
+      <c r="J11" s="1" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="G12" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="H12" s="1" t="s">
-        <v>24</v>
+      <c r="H12" s="1" t="n">
+        <v>1</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="K12" s="4"/>
-      <c r="L12" s="4"/>
-      <c r="M12" s="4"/>
+        <v>25</v>
+      </c>
+      <c r="J12" s="1" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="n">
         <v>1</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="K13" s="4"/>
-      <c r="L13" s="4"/>
-      <c r="M13" s="4"/>
+        <v>27</v>
+      </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="n">
         <v>3</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="G14" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="H14" s="1" t="s">
-        <v>5</v>
+        <v>15</v>
+      </c>
+      <c r="H14" s="1" t="n">
+        <v>1</v>
       </c>
       <c r="I14" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="K14" s="4"/>
-      <c r="L14" s="5"/>
-      <c r="M14" s="5"/>
+        <v>6</v>
+      </c>
+      <c r="J14" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="M14" s="4"/>
+      <c r="N14" s="4"/>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="n">
         <v>2</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="K15" s="4"/>
-      <c r="L15" s="5"/>
-      <c r="M15" s="5"/>
+        <v>9</v>
+      </c>
+      <c r="M15" s="4"/>
+      <c r="N15" s="4"/>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="n">
         <v>1</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="G16" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="H16" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="H16" s="1" t="s">
-        <v>28</v>
-      </c>
       <c r="I16" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="K16" s="4"/>
-      <c r="L16" s="4"/>
-      <c r="M16" s="4"/>
+        <v>29</v>
+      </c>
+      <c r="J16" s="1" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="n">
         <v>1</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="G17" s="1" t="n">
+        <v>31</v>
+      </c>
+      <c r="H17" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="H17" s="1" t="s">
-        <v>31</v>
-      </c>
       <c r="I17" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="K17" s="4"/>
-      <c r="L17" s="4"/>
-      <c r="M17" s="4"/>
+        <v>32</v>
+      </c>
+      <c r="J17" s="1" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="n">
@@ -631,21 +602,21 @@
         <v>500</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="G20" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="H20" s="1" t="s">
-        <v>34</v>
+      <c r="H20" s="1" t="n">
+        <v>2</v>
       </c>
       <c r="I20" s="1" t="s">
-        <v>8</v>
+        <v>35</v>
+      </c>
+      <c r="J20" s="1" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -653,22 +624,22 @@
         <v>1</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="G21" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="H21" s="1" t="s">
-        <v>18</v>
+        <v>36</v>
+      </c>
+      <c r="H21" s="1" t="n">
+        <v>2</v>
       </c>
       <c r="I21" s="1" t="s">
-        <v>8</v>
+        <v>19</v>
+      </c>
+      <c r="J21" s="1" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -676,19 +647,19 @@
         <v>1</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="G22" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="H22" s="1" t="s">
-        <v>36</v>
+        <v>9</v>
+      </c>
+      <c r="H22" s="1" t="n">
+        <v>1</v>
       </c>
       <c r="I22" s="1" t="s">
-        <v>8</v>
+        <v>37</v>
+      </c>
+      <c r="J22" s="1" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -696,10 +667,10 @@
         <v>1</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -707,19 +678,19 @@
         <v>1</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="G24" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="H24" s="1" t="s">
-        <v>37</v>
+        <v>9</v>
+      </c>
+      <c r="H24" s="1" t="n">
+        <v>2</v>
       </c>
       <c r="I24" s="1" t="s">
-        <v>8</v>
+        <v>38</v>
+      </c>
+      <c r="J24" s="1" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -727,51 +698,51 @@
         <v>1</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="G26" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="H26" s="1" t="s">
         <v>41</v>
       </c>
+      <c r="H26" s="1" t="n">
+        <v>2</v>
+      </c>
       <c r="I26" s="1" t="s">
-        <v>14</v>
+        <v>42</v>
+      </c>
+      <c r="J26" s="1" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C27" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="G27" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="H27" s="1" t="s">
         <v>43</v>
       </c>
+      <c r="H27" s="1" t="n">
+        <v>1</v>
+      </c>
       <c r="I27" s="1" t="s">
-        <v>14</v>
+        <v>44</v>
+      </c>
+      <c r="J27" s="1" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C28" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C29" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C30" s="1" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
   </sheetData>

</xml_diff>